<commit_message>
changes on main code, fill entries function, Excel file saving function
</commit_message>
<xml_diff>
--- a/Sauvegarde-Archive/Archive_de_l'employee_ABDALLAH MAHAMAT YAHAYA.xlsx
+++ b/Sauvegarde-Archive/Archive_de_l'employee_ABDALLAH MAHAMAT YAHAYA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maman Sani Ibrahim\Documents\HCi3N Job Time Calculator\Sauvegarde-Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18C012E-B65C-41D4-8BF9-F9ACD679B9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C258B5-832F-405E-8A4B-EC72C93F00E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -231,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -242,23 +242,21 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,8 +605,8 @@
   </sheetPr>
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,36 +625,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="150" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="12" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:12" ht="22.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -1034,30 +1032,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
       <c r="J17" s="8">
         <f>SUM(J4:J16)</f>
         <v>5.145833333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="J19" s="15"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -1437,17 +1435,17 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
       <c r="J33" s="8">
         <f>SUM(J20:J32)</f>
         <v>4.8958333333333339</v>
@@ -1462,7 +1460,7 @@
     <mergeCell ref="A33:I33"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>